<commit_message>
uploading final draft for python HW submission
</commit_message>
<xml_diff>
--- a/Resources/budget_data - Copy.xlsx
+++ b/Resources/budget_data - Copy.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\azbir\LearnPython\python-challenge\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E0F68FE0-1484-440F-A717-BA4079DB7137}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B6EC4A-7CED-4A2A-9920-85EEC5C74407}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11412" yWindow="132" windowWidth="11544" windowHeight="12228"/>
+    <workbookView xWindow="1710" yWindow="66" windowWidth="18162" windowHeight="12228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="budget_data - Copy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -45,11 +52,17 @@
   <si>
     <t>Greatest Decrease</t>
   </si>
+  <si>
+    <t>Index Position</t>
+  </si>
+  <si>
+    <t>index starts with zero; change has no value in the 10-Jan, so the max is in position 24</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
@@ -890,11 +903,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C94"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -902,7 +915,7 @@
     <col min="3" max="3" width="11.20703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -912,16 +925,22 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>43475</v>
       </c>
       <c r="B2">
         <v>867884</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>43506</v>
       </c>
@@ -932,8 +951,12 @@
         <f>B3-B2</f>
         <v>116771</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E3">
+        <f>E2+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>43534</v>
       </c>
@@ -944,8 +967,12 @@
         <f t="shared" ref="C4:C67" si="0">B4-B3</f>
         <v>-662642</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4">
+        <f t="shared" ref="E4:E27" si="1">E3+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>43565</v>
       </c>
@@ -956,8 +983,12 @@
         <f t="shared" si="0"/>
         <v>-391430</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>43595</v>
       </c>
@@ -968,8 +999,12 @@
         <f t="shared" si="0"/>
         <v>379920</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>43626</v>
       </c>
@@ -980,8 +1015,12 @@
         <f t="shared" si="0"/>
         <v>212354</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>43656</v>
       </c>
@@ -992,8 +1031,12 @@
         <f t="shared" si="0"/>
         <v>510239</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>43687</v>
       </c>
@@ -1004,8 +1047,12 @@
         <f t="shared" si="0"/>
         <v>-428211</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>43718</v>
       </c>
@@ -1016,8 +1063,12 @@
         <f t="shared" si="0"/>
         <v>-821271</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>43748</v>
       </c>
@@ -1028,8 +1079,12 @@
         <f t="shared" si="0"/>
         <v>693918</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>43779</v>
       </c>
@@ -1040,8 +1095,12 @@
         <f t="shared" si="0"/>
         <v>416278</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>43809</v>
       </c>
@@ -1052,8 +1111,12 @@
         <f t="shared" si="0"/>
         <v>-974163</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>43476</v>
       </c>
@@ -1064,8 +1127,12 @@
         <f t="shared" si="0"/>
         <v>860159</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>43507</v>
       </c>
@@ -1076,8 +1143,12 @@
         <f t="shared" si="0"/>
         <v>-1115009</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>43535</v>
       </c>
@@ -1088,8 +1159,12 @@
         <f t="shared" si="0"/>
         <v>1033048</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1">
         <v>43566</v>
       </c>
@@ -1100,8 +1175,12 @@
         <f t="shared" si="0"/>
         <v>95318</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1">
         <v>43596</v>
       </c>
@@ -1112,8 +1191,12 @@
         <f t="shared" si="0"/>
         <v>-308093</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1">
         <v>43627</v>
       </c>
@@ -1124,8 +1207,12 @@
         <f t="shared" si="0"/>
         <v>99052</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1">
         <v>43657</v>
       </c>
@@ -1136,8 +1223,12 @@
         <f t="shared" si="0"/>
         <v>-521393</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1">
         <v>43688</v>
       </c>
@@ -1148,8 +1239,12 @@
         <f t="shared" si="0"/>
         <v>605450</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1">
         <v>43719</v>
       </c>
@@ -1160,8 +1255,12 @@
         <f t="shared" si="0"/>
         <v>231727</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1">
         <v>43749</v>
       </c>
@@ -1172,8 +1271,12 @@
         <f t="shared" si="0"/>
         <v>-65187</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1">
         <v>43780</v>
       </c>
@@ -1184,8 +1287,12 @@
         <f t="shared" si="0"/>
         <v>-702716</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1">
         <v>43810</v>
       </c>
@@ -1196,8 +1303,12 @@
         <f t="shared" si="0"/>
         <v>177975</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1">
         <v>43477</v>
       </c>
@@ -1208,8 +1319,15 @@
         <f t="shared" si="0"/>
         <v>-1065544</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="G26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1">
         <v>43508</v>
       </c>
@@ -1220,8 +1338,12 @@
         <f t="shared" si="0"/>
         <v>1926159</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1">
         <v>43536</v>
       </c>
@@ -1233,7 +1355,7 @@
         <v>-917805</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1">
         <v>43567</v>
       </c>
@@ -1245,7 +1367,7 @@
         <v>898730</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1">
         <v>43597</v>
       </c>
@@ -1257,7 +1379,7 @@
         <v>-334262</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1">
         <v>43628</v>
       </c>
@@ -1269,7 +1391,7 @@
         <v>-246499</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1">
         <v>43658</v>
       </c>
@@ -1709,7 +1831,7 @@
         <v>423389</v>
       </c>
       <c r="C68">
-        <f t="shared" ref="C68:C87" si="1">B68-B67</f>
+        <f t="shared" ref="C68:C87" si="2">B68-B67</f>
         <v>335594</v>
       </c>
     </row>
@@ -1721,7 +1843,7 @@
         <v>840723</v>
       </c>
       <c r="C69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>417334</v>
       </c>
     </row>
@@ -1733,7 +1855,7 @@
         <v>568529</v>
       </c>
       <c r="C70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-272194</v>
       </c>
     </row>
@@ -1745,7 +1867,7 @@
         <v>332067</v>
       </c>
       <c r="C71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-236462</v>
       </c>
     </row>
@@ -1757,7 +1879,7 @@
         <v>989499</v>
       </c>
       <c r="C72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>657432</v>
       </c>
     </row>
@@ -1769,7 +1891,7 @@
         <v>778237</v>
       </c>
       <c r="C73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-211262</v>
       </c>
     </row>
@@ -1781,7 +1903,7 @@
         <v>650000</v>
       </c>
       <c r="C74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-128237</v>
       </c>
     </row>
@@ -1793,7 +1915,7 @@
         <v>-1100387</v>
       </c>
       <c r="C75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1750387</v>
       </c>
     </row>
@@ -1805,7 +1927,7 @@
         <v>-174946</v>
       </c>
       <c r="C76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>925441</v>
       </c>
     </row>
@@ -1817,7 +1939,7 @@
         <v>757143</v>
       </c>
       <c r="C77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>932089</v>
       </c>
     </row>
@@ -1829,7 +1951,7 @@
         <v>445709</v>
       </c>
       <c r="C78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-311434</v>
       </c>
     </row>
@@ -1841,7 +1963,7 @@
         <v>712961</v>
       </c>
       <c r="C79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>267252</v>
       </c>
     </row>
@@ -1853,7 +1975,7 @@
         <v>-1163797</v>
       </c>
       <c r="C80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-1876758</v>
       </c>
     </row>
@@ -1865,7 +1987,7 @@
         <v>569899</v>
       </c>
       <c r="C81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1733696</v>
       </c>
     </row>
@@ -1877,7 +1999,7 @@
         <v>768450</v>
       </c>
       <c r="C82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>198551</v>
       </c>
     </row>
@@ -1889,7 +2011,7 @@
         <v>102685</v>
       </c>
       <c r="C83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-665765</v>
       </c>
     </row>
@@ -1901,7 +2023,7 @@
         <v>795914</v>
       </c>
       <c r="C84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>693229</v>
       </c>
     </row>
@@ -1913,7 +2035,7 @@
         <v>60988</v>
       </c>
       <c r="C85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-734926</v>
       </c>
     </row>
@@ -1925,7 +2047,7 @@
         <v>138230</v>
       </c>
       <c r="C86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>77242</v>
       </c>
     </row>
@@ -1937,7 +2059,7 @@
         <v>671099</v>
       </c>
       <c r="C87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>532869</v>
       </c>
     </row>

</xml_diff>